<commit_message>
Using plotly for interactive plots
</commit_message>
<xml_diff>
--- a/data/AES42_Tempo_2011.xlsx
+++ b/data/AES42_Tempo_2011.xlsx
@@ -92,10 +92,10 @@
     <t xml:space="preserve">Dix_trac</t>
   </si>
   <si>
-    <t xml:space="preserve">Klap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sche</t>
+    <t xml:space="preserve">Klapuri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scheirer</t>
   </si>
   <si>
     <t xml:space="preserve">Tzan_hist</t>
@@ -1769,8 +1769,8 @@
   </sheetPr>
   <dimension ref="A1:Y466"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>